<commit_message>
change report for lab2
</commit_message>
<xml_diff>
--- a/cloud/lab2/Azure lab team 3.xlsx
+++ b/cloud/lab2/Azure lab team 3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C984319-CE7B-46C8-A4B3-A1CB19AA3481}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658601A9-1A2C-4521-8A1F-4992C2B3FD85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="177">
   <si>
     <t>IT Tower</t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>Virtual Machines Usage</t>
+  </si>
+  <si>
+    <t>Standard Emotion API</t>
   </si>
 </sst>
 </file>
@@ -944,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989C0B6A-CB7C-4C40-AC78-34258AA2DBC4}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,7 +1413,7 @@
         <v>37</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>37</v>

</xml_diff>